<commit_message>
Funciones Logicas y Estadisticas con DB
</commit_message>
<xml_diff>
--- a/db_supermercado.xlsx
+++ b/db_supermercado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\xav-m15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4564CB-1DFF-48EC-96DF-8407267AD379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFD7DEA-973A-4B23-9D77-36FF65E7D388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10800" activeTab="1" xr2:uid="{97DD950F-96E2-4B97-B3BD-DF46440A712E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10800" activeTab="2" xr2:uid="{97DD950F-96E2-4B97-B3BD-DF46440A712E}"/>
   </bookViews>
   <sheets>
     <sheet name="ventas" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,10 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">regiones!$A$1:$A$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">vendedores!$A$1:$A$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ventas!$A$1:$G$181</definedName>
+    <definedName name="condicion_premio">vendedores!$K$2</definedName>
     <definedName name="db_condicion">estadisticas!$A$1:$G$2</definedName>
+    <definedName name="premio_f">vendedores!$M$2</definedName>
+    <definedName name="premio_v">vendedores!$L$2</definedName>
     <definedName name="tabla_ventas">ventas!$A:$G</definedName>
     <definedName name="ventas_precio">ventas!$F:$F</definedName>
     <definedName name="ventas_producto">ventas!$C:$C</definedName>
@@ -51,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="54">
   <si>
     <t>Mes</t>
   </si>
@@ -187,6 +190,33 @@
   <si>
     <t>Cantidad</t>
   </si>
+  <si>
+    <t>Recaudacion</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>comision</t>
+  </si>
+  <si>
+    <t>premio</t>
+  </si>
+  <si>
+    <t>condicion</t>
+  </si>
+  <si>
+    <t>OBJ</t>
+  </si>
+  <si>
+    <t>COMISION</t>
+  </si>
 </sst>
 </file>
 
@@ -195,9 +225,9 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +241,14 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -241,12 +279,22 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Millares" xfId="2" builtinId="3"/>
@@ -254,7 +302,568 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{385567CA-A40D-4706-8194-05E7B43A981C}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="49">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -265,6 +874,95 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6EB613B6-93C3-4B79-B71A-B48B318AD25F}" name="tabla_vendedores" displayName="tabla_vendedores" ref="A1:I8" totalsRowCount="1" headerRowDxfId="47" dataDxfId="48" dataCellStyle="Moneda">
+  <autoFilter ref="A1:I7" xr:uid="{6EB613B6-93C3-4B79-B71A-B48B318AD25F}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{651BE219-A1EF-48C4-819B-EDF17E87C710}" name="Vendedor" totalsRowLabel="Total" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{A0C0EC34-1BF3-4A8D-B963-A1D242E2D48A}" name="Antioquia" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="7" dataCellStyle="Moneda"/>
+    <tableColumn id="3" xr3:uid="{D49F2007-032B-4FEA-92E8-0C12E5209E43}" name="Caribe" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="6" dataCellStyle="Moneda"/>
+    <tableColumn id="4" xr3:uid="{016A324D-F516-42E9-AAB8-258A3E0934E6}" name="Central" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="5" dataCellStyle="Moneda"/>
+    <tableColumn id="5" xr3:uid="{2F122157-D17A-4E5E-A738-1132F3278694}" name="Pacifico" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="4" dataCellStyle="Moneda"/>
+    <tableColumn id="6" xr3:uid="{F80876AC-A4F3-4C96-B28C-9A64096BDAE3}" name="Santanderes" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="3" dataCellStyle="Moneda"/>
+    <tableColumn id="7" xr3:uid="{E4A90127-FD5D-40F2-971C-8791F04CB5AE}" name="total" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{52643D21-F702-47F2-9158-83252F366678}" name="COMISION" totalsRowFunction="average" dataDxfId="9" totalsRowDxfId="1" dataCellStyle="Moneda">
+      <calculatedColumnFormula>IF(tabla_vendedores[[#This Row],[total]]&gt;=condicion_premio,tabla_vendedores[[#This Row],[total]]*premio_v,tabla_vendedores[[#This Row],[total]]*premio_f)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{B84C3849-3836-444B-AEF1-E508B0624FBC}" name="OBJ" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="0">
+      <calculatedColumnFormula>IF(tabla_vendedores[[#This Row],[total]]&gt;=condicion_premio,"SI","NO")</calculatedColumnFormula>
+      <totalsRowFormula>COUNTIF(tabla_vendedores[OBJ],"SI")</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{022CD2BF-05BB-43A8-9448-1DA88C404803}" name="tabla_productos" displayName="tabla_productos" ref="A1:H7" totalsRowCount="1" headerRowDxfId="45">
+  <autoFilter ref="A1:H6" xr:uid="{022CD2BF-05BB-43A8-9448-1DA88C404803}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{6C663D01-F8B2-4795-83BA-31076894C9BB}" name="Producto" totalsRowLabel="Total" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{18359577-D30A-46C5-936A-9E30967F2919}" name="Capioli" totalsRowFunction="sum" totalsRowDxfId="40" dataCellStyle="Moneda">
+      <calculatedColumnFormula>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,B$1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{A67D2298-61F8-46CC-A412-EA57C271ED3A}" name="Cardenas" totalsRowFunction="sum" dataDxfId="44" totalsRowDxfId="39">
+      <calculatedColumnFormula>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,C$1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{028643E8-331C-4446-9168-B209480993CD}" name="Juarez" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="38">
+      <calculatedColumnFormula>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,D$1)</calculatedColumnFormula>
+      <totalsRowFormula>SUBTOTAL(109,tabla_productos[Cardenas])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{D211A275-C157-44F2-9637-DAE6202A09E7}" name="Lujan" totalsRowFunction="custom" dataDxfId="42" totalsRowDxfId="37">
+      <calculatedColumnFormula>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,E$1)</calculatedColumnFormula>
+      <totalsRowFormula>SUBTOTAL(109,tabla_productos[Juarez])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{9ACEDA62-DF4D-4139-93D5-33CF4B68746E}" name="Sanchez" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="36">
+      <calculatedColumnFormula>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,F$1)</calculatedColumnFormula>
+      <totalsRowFormula>SUBTOTAL(109,tabla_productos[Juarez])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{19A365D1-DD42-4C49-AEC8-BCC07389F228}" name="Zuloaga" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="35">
+      <calculatedColumnFormula>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,G$1)</calculatedColumnFormula>
+      <totalsRowFormula>SUBTOTAL(109,tabla_productos[Lujan])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{7023D789-0747-460D-9501-A04FDB40E412}" name="Total" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="34">
+      <calculatedColumnFormula>SUM(tabla_productos[[#This Row],[Capioli]:[Zuloaga]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4918B505-8171-4743-8C7C-9EA7D0478895}" name="tabla_regiones" displayName="tabla_regiones" ref="A1:H7" totalsRowCount="1">
+  <autoFilter ref="A1:H6" xr:uid="{4918B505-8171-4743-8C7C-9EA7D0478895}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{2638D21F-4166-4706-ABAF-2871C1BA3138}" name="Region" totalsRowLabel="Total" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{6685E649-A14C-41A0-BBB3-709D1B6D37F7}" name="Capioli" totalsRowFunction="sum" dataDxfId="30" totalsRowDxfId="23" dataCellStyle="Moneda">
+      <calculatedColumnFormula>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,B$1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{0CB22250-B691-42D0-A3A6-11404C0187BA}" name="Cardenas" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="22">
+      <calculatedColumnFormula>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,C$1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{2907BCD5-1B9C-447F-9385-C09BF56FFF75}" name="Juarez" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="21" dataCellStyle="Moneda">
+      <calculatedColumnFormula>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,D$1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{1B2EEB25-DE9E-4AA6-BE30-30925CE712EA}" name="Lujan" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="20">
+      <calculatedColumnFormula>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,E$1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{973093B2-522D-4119-83AE-9553448A1F3D}" name="Sanchez" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="19" dataCellStyle="Moneda">
+      <calculatedColumnFormula>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,F$1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{E7756FE0-44BE-4F87-BB31-FF5AEF36F1FC}" name="Zuloaga" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="18">
+      <calculatedColumnFormula>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,G$1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{859C5AC2-7E69-40FF-9FF2-14674C44A2D1}" name="Total" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="17">
+      <calculatedColumnFormula>SUM(tabla_regiones[[#This Row],[Capioli]:[Zuloaga]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -564,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D73896-876D-4E2F-AA30-36383BB76670}">
-  <dimension ref="A1:K181"/>
+  <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView topLeftCell="H2" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +1375,7 @@
       </c>
       <c r="K3" s="3">
         <f>MAX(ventas_precio)</f>
-        <v>31939624</v>
+        <v>50835211</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -707,11 +1405,11 @@
       </c>
       <c r="J4" s="4">
         <f>AVERAGE(ventas_unidades)</f>
-        <v>2907.2277777777776</v>
+        <v>2906.6906077348067</v>
       </c>
       <c r="K4" s="3">
         <f>AVERAGE(ventas_precio)</f>
-        <v>17796672.055555556</v>
+        <v>17979205.419889502</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -741,11 +1439,11 @@
       </c>
       <c r="J5">
         <f>MEDIAN(ventas_unidades)</f>
-        <v>2930.5</v>
+        <v>2925</v>
       </c>
       <c r="K5" s="3">
         <f>MEDIAN(ventas_precio)</f>
-        <v>17980831.5</v>
+        <v>18002618</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -775,11 +1473,11 @@
       </c>
       <c r="J6" s="2">
         <f>SUM(ventas_unidades)</f>
-        <v>523301</v>
+        <v>526111</v>
       </c>
       <c r="K6" s="3">
         <f>SUM(ventas_precio)</f>
-        <v>3203400970</v>
+        <v>3254236181</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -4805,6 +5503,29 @@
       </c>
       <c r="G181" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B182" s="1">
+        <v>2011</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E182" s="2">
+        <v>2810</v>
+      </c>
+      <c r="F182" s="3">
+        <v>50835211</v>
+      </c>
+      <c r="G182" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -4855,15 +5576,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0B1BE0-A402-4B19-A730-4404D220FBC4}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4891,7 +5618,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="B2" s="6"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
@@ -4899,46 +5626,97 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4">
-        <f>DMIN(tabla_ventas,ventas!E1,db_condicion)</f>
-        <v>928</v>
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="B5" s="2">
+        <f>DMIN(ventas!A:G,ventas!E1,db_condicion)</f>
+        <v>928</v>
+      </c>
+      <c r="C5" s="3">
+        <f>DMIN(ventas!$A:$G,ventas!$F$1,db_condicion)</f>
+        <v>5090135</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="B6" s="2">
+        <f>DMAX(ventas!A:G,ventas!E1,db_condicion)</f>
+        <v>4991</v>
+      </c>
+      <c r="C6" s="3">
+        <f>DMAX(ventas!$A:$G,ventas!$F$1,db_condicion)</f>
+        <v>50835211</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="B7" s="2">
+        <f>DCOUNT(ventas!$A:$G,ventas!E1,$A$1:$G$2)</f>
+        <v>181</v>
+      </c>
+      <c r="C7" s="2">
+        <f>DCOUNT(ventas!$A:$G,ventas!$F$1,db_condicion)</f>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="5">
+        <f>DAVERAGE(ventas!A:G,ventas!$E$1,db_condicion)</f>
+        <v>2906.6906077348067</v>
+      </c>
+      <c r="C8" s="3">
+        <f>DAVERAGE(ventas!$A:$G,ventas!$F$1,db_condicion)</f>
+        <v>17979205.419889502</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>39</v>
+      </c>
+      <c r="B9" s="2">
+        <f>DSUM(ventas!A:G,ventas!$E$1,db_condicion)</f>
+        <v>526111</v>
+      </c>
+      <c r="C9" s="3">
+        <f>DSUM(ventas!$A:$G,ventas!$F$1,db_condicion)</f>
+        <v>3254236181</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F2" xr:uid="{657C0106-0F2E-45D9-AA72-68CB48D0ECAB}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F3" xr:uid="{657C0106-0F2E-45D9-AA72-68CB48D0ECAB}">
       <formula1>1</formula1>
       <formula2>99999999</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E2" xr:uid="{36656274-6FF5-4EB6-97BF-D11D7BF4E074}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E3" xr:uid="{36656274-6FF5-4EB6-97BF-D11D7BF4E074}">
       <formula1>1</formula1>
       <formula2>999999999</formula2>
     </dataValidation>
@@ -4951,19 +5729,19 @@
           <x14:formula1>
             <xm:f>regiones!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G2</xm:sqref>
+          <xm:sqref>G1:G3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8CBA7C05-79CC-4F55-A869-19AFFBA52CAC}">
           <x14:formula1>
             <xm:f>vendedores!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D1:D2</xm:sqref>
+          <xm:sqref>D1:D3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A984AE60-5ADE-4721-A018-8C11FB45850C}">
           <x14:formula1>
             <xm:f>productos!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C2</xm:sqref>
+          <xm:sqref>C1:C3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4973,77 +5751,354 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD817869-3332-4BA1-9CA6-D67763739E2F}">
-  <dimension ref="A1:A181"/>
+  <dimension ref="A1:M181"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A2,ventas_region,B$1)</f>
+        <v>73836463</v>
+      </c>
+      <c r="C2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A2,ventas_region,C$1)</f>
+        <v>76700859</v>
+      </c>
+      <c r="D2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A2,ventas_region,D$1)</f>
+        <v>44881356</v>
+      </c>
+      <c r="E2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A2,ventas_region,E$1)</f>
+        <v>135280108</v>
+      </c>
+      <c r="F2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A2,ventas_region,F$1)</f>
+        <v>27153333</v>
+      </c>
+      <c r="G2" s="10">
+        <f>SUM($B2:$F2)</f>
+        <v>357852119</v>
+      </c>
+      <c r="H2" s="3">
+        <f>IF(tabla_vendedores[[#This Row],[total]]&gt;=condicion_premio,tabla_vendedores[[#This Row],[total]]*premio_v,tabla_vendedores[[#This Row],[total]]*premio_f)</f>
+        <v>35785211.899999999</v>
+      </c>
+      <c r="I2" s="10" t="str">
+        <f>IF(tabla_vendedores[[#This Row],[total]]&gt;=condicion_premio,"SI","NO")</f>
+        <v>NO</v>
+      </c>
+      <c r="K2" s="5">
+        <v>600000000</v>
+      </c>
+      <c r="L2" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="M2" s="11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A3,ventas_region,B$1)</f>
+        <v>169977929</v>
+      </c>
+      <c r="C3" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A3,ventas_region,C$1)</f>
+        <v>71950539</v>
+      </c>
+      <c r="D3" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A3,ventas_region,D$1)</f>
+        <v>52631529</v>
+      </c>
+      <c r="E3" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A3,ventas_region,E$1)</f>
+        <v>109144041</v>
+      </c>
+      <c r="F3" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A3,ventas_region,F$1)</f>
+        <v>232698504</v>
+      </c>
+      <c r="G3" s="10">
+        <f t="shared" ref="G3:G7" si="0">SUM($B3:$F3)</f>
+        <v>636402542</v>
+      </c>
+      <c r="H3" s="3">
+        <f>IF(tabla_vendedores[[#This Row],[total]]&gt;=condicion_premio,tabla_vendedores[[#This Row],[total]]*premio_v,tabla_vendedores[[#This Row],[total]]*premio_f)</f>
+        <v>159100635.5</v>
+      </c>
+      <c r="I3" s="10" t="str">
+        <f>IF(tabla_vendedores[[#This Row],[total]]&gt;=condicion_premio,"SI","NO")</f>
+        <v>SI</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A4,ventas_region,B$1)</f>
+        <v>336034466</v>
+      </c>
+      <c r="C4" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A4,ventas_region,C$1)</f>
+        <v>110517698</v>
+      </c>
+      <c r="D4" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A4,ventas_region,D$1)</f>
+        <v>93604609</v>
+      </c>
+      <c r="E4" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A4,ventas_region,E$1)</f>
+        <v>94535993</v>
+      </c>
+      <c r="F4" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A4,ventas_region,F$1)</f>
+        <v>77744662</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" si="0"/>
+        <v>712437428</v>
+      </c>
+      <c r="H4" s="3">
+        <f>IF(tabla_vendedores[[#This Row],[total]]&gt;=condicion_premio,tabla_vendedores[[#This Row],[total]]*premio_v,tabla_vendedores[[#This Row],[total]]*premio_f)</f>
+        <v>178109357</v>
+      </c>
+      <c r="I4" s="10" t="str">
+        <f>IF(tabla_vendedores[[#This Row],[total]]&gt;=condicion_premio,"SI","NO")</f>
+        <v>SI</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A5,ventas_region,B$1)</f>
+        <v>75839132</v>
+      </c>
+      <c r="C5" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A5,ventas_region,C$1)</f>
+        <v>88920515</v>
+      </c>
+      <c r="D5" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A5,ventas_region,D$1)</f>
+        <v>271532147</v>
+      </c>
+      <c r="E5" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A5,ventas_region,E$1)</f>
+        <v>193222871</v>
+      </c>
+      <c r="F5" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A5,ventas_region,F$1)</f>
+        <v>131950052</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" si="0"/>
+        <v>761464717</v>
+      </c>
+      <c r="H5" s="3">
+        <f>IF(tabla_vendedores[[#This Row],[total]]&gt;=condicion_premio,tabla_vendedores[[#This Row],[total]]*premio_v,tabla_vendedores[[#This Row],[total]]*premio_f)</f>
+        <v>190366179.25</v>
+      </c>
+      <c r="I5" s="10" t="str">
+        <f>IF(tabla_vendedores[[#This Row],[total]]&gt;=condicion_premio,"SI","NO")</f>
+        <v>SI</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A6,ventas_region,B$1)</f>
+        <v>16585017</v>
+      </c>
+      <c r="C6" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A6,ventas_region,C$1)</f>
+        <v>275641384</v>
+      </c>
+      <c r="D6" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A6,ventas_region,D$1)</f>
+        <v>50806730</v>
+      </c>
+      <c r="E6" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A6,ventas_region,E$1)</f>
+        <v>48593995</v>
+      </c>
+      <c r="F6" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A6,ventas_region,F$1)</f>
+        <v>167729464</v>
+      </c>
+      <c r="G6" s="10">
+        <f t="shared" si="0"/>
+        <v>559356590</v>
+      </c>
+      <c r="H6" s="3">
+        <f>IF(tabla_vendedores[[#This Row],[total]]&gt;=condicion_premio,tabla_vendedores[[#This Row],[total]]*premio_v,tabla_vendedores[[#This Row],[total]]*premio_f)</f>
+        <v>55935659</v>
+      </c>
+      <c r="I6" s="10" t="str">
+        <f>IF(tabla_vendedores[[#This Row],[total]]&gt;=condicion_premio,"SI","NO")</f>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A7,ventas_region,B$1)</f>
+        <v>31378227</v>
+      </c>
+      <c r="C7" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A7,ventas_region,C$1)</f>
+        <v>31867112</v>
+      </c>
+      <c r="D7" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A7,ventas_region,D$1)</f>
+        <v>63246530</v>
+      </c>
+      <c r="E7" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A7,ventas_region,E$1)</f>
+        <v>59797810</v>
+      </c>
+      <c r="F7" s="3">
+        <f>SUMIFS(ventas_precio,ventas_vendedor,$A7,ventas_region,F$1)</f>
+        <v>40433106</v>
+      </c>
+      <c r="G7" s="10">
+        <f t="shared" si="0"/>
+        <v>226722785</v>
+      </c>
+      <c r="H7" s="3">
+        <f>IF(tabla_vendedores[[#This Row],[total]]&gt;=condicion_premio,tabla_vendedores[[#This Row],[total]]*premio_v,tabla_vendedores[[#This Row],[total]]*premio_f)</f>
+        <v>22672278.5</v>
+      </c>
+      <c r="I7" s="10" t="str">
+        <f>IF(tabla_vendedores[[#This Row],[total]]&gt;=condicion_premio,"SI","NO")</f>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="10">
+        <f>SUBTOTAL(109,tabla_vendedores[Antioquia])</f>
+        <v>703651234</v>
+      </c>
+      <c r="C8" s="10">
+        <f>SUBTOTAL(109,tabla_vendedores[Caribe])</f>
+        <v>655598107</v>
+      </c>
+      <c r="D8" s="10">
+        <f>SUBTOTAL(109,tabla_vendedores[Central])</f>
+        <v>576702901</v>
+      </c>
+      <c r="E8" s="10">
+        <f>SUBTOTAL(109,tabla_vendedores[Pacifico])</f>
+        <v>640574818</v>
+      </c>
+      <c r="F8" s="10">
+        <f>SUBTOTAL(109,tabla_vendedores[Santanderes])</f>
+        <v>677709121</v>
+      </c>
+      <c r="G8" s="10">
+        <f>SUBTOTAL(109,tabla_vendedores[total])</f>
+        <v>3254236181</v>
+      </c>
+      <c r="H8" s="10">
+        <f>SUBTOTAL(101,tabla_vendedores[COMISION])</f>
+        <v>106994886.85833333</v>
+      </c>
+      <c r="I8" s="12">
+        <f>COUNTIF(tabla_vendedores[OBJ],"SI")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -5542,84 +6597,290 @@
       <c r="A181"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A7" xr:uid="{CD817869-3332-4BA1-9CA6-D67763739E2F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A7">
-      <sortCondition ref="A1:A7"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F705A57D-BFD6-4730-9DEF-9553A00DFEA3}">
+          <x14:formula1>
+            <xm:f>regiones!$A$2:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:F1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD42545-9B5A-464E-80B4-01A7EF327B8D}">
-  <dimension ref="A1:A181"/>
+  <dimension ref="A1:H182"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,B$1)</f>
+        <v>186115319</v>
+      </c>
+      <c r="C2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,C$1)</f>
+        <v>109144041</v>
+      </c>
+      <c r="D2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,D$1)</f>
+        <v>94535993</v>
+      </c>
+      <c r="E2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,E$1)</f>
+        <v>193222871</v>
+      </c>
+      <c r="F2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,F$1)</f>
+        <v>48593995</v>
+      </c>
+      <c r="G2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,G$1)</f>
+        <v>59797810</v>
+      </c>
+      <c r="H2" s="10">
+        <f>SUM(tabla_productos[[#This Row],[Capioli]:[Zuloaga]])</f>
+        <v>691410029</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,B$1)</f>
+        <v>27153333</v>
+      </c>
+      <c r="C3" s="7">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,C$1)</f>
+        <v>232698504</v>
+      </c>
+      <c r="D3" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,D$1)</f>
+        <v>77744662</v>
+      </c>
+      <c r="E3" s="7">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,E$1)</f>
+        <v>131950052</v>
+      </c>
+      <c r="F3" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,F$1)</f>
+        <v>167729464</v>
+      </c>
+      <c r="G3" s="7">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,G$1)</f>
+        <v>40433106</v>
+      </c>
+      <c r="H3" s="10">
+        <f>SUM(tabla_productos[[#This Row],[Capioli]:[Zuloaga]])</f>
+        <v>677709121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,B$1)</f>
+        <v>76700859</v>
+      </c>
+      <c r="C4" s="7">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,C$1)</f>
+        <v>71950539</v>
+      </c>
+      <c r="D4" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,D$1)</f>
+        <v>110517698</v>
+      </c>
+      <c r="E4" s="7">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,E$1)</f>
+        <v>88920515</v>
+      </c>
+      <c r="F4" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,F$1)</f>
+        <v>275641384</v>
+      </c>
+      <c r="G4" s="7">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,G$1)</f>
+        <v>31867112</v>
+      </c>
+      <c r="H4" s="10">
+        <f>SUM(tabla_productos[[#This Row],[Capioli]:[Zuloaga]])</f>
+        <v>655598107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,B$1)</f>
+        <v>23001252</v>
+      </c>
+      <c r="C5" s="7">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,C$1)</f>
+        <v>169977929</v>
+      </c>
+      <c r="D5" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,D$1)</f>
+        <v>336034466</v>
+      </c>
+      <c r="E5" s="7">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,E$1)</f>
+        <v>75839132</v>
+      </c>
+      <c r="F5" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,F$1)</f>
+        <v>16585017</v>
+      </c>
+      <c r="G5" s="7">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,G$1)</f>
+        <v>31378227</v>
+      </c>
+      <c r="H5" s="10">
+        <f>SUM(tabla_productos[[#This Row],[Capioli]:[Zuloaga]])</f>
+        <v>652816023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,B$1)</f>
+        <v>44881356</v>
+      </c>
+      <c r="C6" s="7">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,C$1)</f>
+        <v>52631529</v>
+      </c>
+      <c r="D6" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,D$1)</f>
+        <v>93604609</v>
+      </c>
+      <c r="E6" s="7">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,E$1)</f>
+        <v>271532147</v>
+      </c>
+      <c r="F6" s="3">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,F$1)</f>
+        <v>50806730</v>
+      </c>
+      <c r="G6" s="7">
+        <f>SUMIFS(ventas_precio,ventas_producto,tabla_productos[[#This Row],[Producto]],ventas_vendedor,G$1)</f>
+        <v>63246530</v>
+      </c>
+      <c r="H6" s="10">
+        <f>SUM(tabla_productos[[#This Row],[Capioli]:[Zuloaga]])</f>
+        <v>576702901</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="9">
+        <f>SUBTOTAL(109,tabla_productos[Capioli])</f>
+        <v>357852119</v>
+      </c>
+      <c r="C7" s="8">
+        <f>SUBTOTAL(109,tabla_productos[Cardenas])</f>
+        <v>636402542</v>
+      </c>
+      <c r="D7" s="9">
+        <f>SUBTOTAL(109,tabla_productos[Cardenas])</f>
+        <v>636402542</v>
+      </c>
+      <c r="E7" s="8">
+        <f>SUBTOTAL(109,tabla_productos[Juarez])</f>
+        <v>712437428</v>
+      </c>
+      <c r="F7" s="9">
+        <f>SUBTOTAL(109,tabla_productos[Juarez])</f>
+        <v>712437428</v>
+      </c>
+      <c r="G7" s="8">
+        <f>SUBTOTAL(109,tabla_productos[Lujan])</f>
+        <v>761464717</v>
+      </c>
+      <c r="H7" s="9">
+        <f>SUBTOTAL(109,tabla_productos[Total])</f>
+        <v>3254236181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -6117,86 +7378,296 @@
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181"/>
     </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:A6" xr:uid="{BBD42545-9B5A-464E-80B4-01A7EF327B8D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A181">
-    <sortCondition ref="A2:A181"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A182">
+    <sortCondition ref="A2:A182"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A19212AC-1343-4D6D-9910-5CA1FF214215}">
+          <x14:formula1>
+            <xm:f>vendedores!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:G1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FA5DA4-F2E8-4268-9AB4-039274B82003}">
-  <dimension ref="A1:A181"/>
+  <dimension ref="A1:H182"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="F2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,B$1)</f>
+        <v>73836463</v>
+      </c>
+      <c r="C2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,C$1)</f>
+        <v>169977929</v>
+      </c>
+      <c r="D2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,D$1)</f>
+        <v>336034466</v>
+      </c>
+      <c r="E2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,E$1)</f>
+        <v>75839132</v>
+      </c>
+      <c r="F2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,F$1)</f>
+        <v>16585017</v>
+      </c>
+      <c r="G2" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,G$1)</f>
+        <v>31378227</v>
+      </c>
+      <c r="H2" s="7">
+        <f>SUM(tabla_regiones[[#This Row],[Capioli]:[Zuloaga]])</f>
+        <v>703651234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,B$1)</f>
+        <v>76700859</v>
+      </c>
+      <c r="C3" s="7">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,C$1)</f>
+        <v>71950539</v>
+      </c>
+      <c r="D3" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,D$1)</f>
+        <v>110517698</v>
+      </c>
+      <c r="E3" s="7">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,E$1)</f>
+        <v>88920515</v>
+      </c>
+      <c r="F3" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,F$1)</f>
+        <v>275641384</v>
+      </c>
+      <c r="G3" s="7">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,G$1)</f>
+        <v>31867112</v>
+      </c>
+      <c r="H3" s="7">
+        <f>SUM(tabla_regiones[[#This Row],[Capioli]:[Zuloaga]])</f>
+        <v>655598107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,B$1)</f>
+        <v>44881356</v>
+      </c>
+      <c r="C4" s="7">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,C$1)</f>
+        <v>52631529</v>
+      </c>
+      <c r="D4" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,D$1)</f>
+        <v>93604609</v>
+      </c>
+      <c r="E4" s="7">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,E$1)</f>
+        <v>271532147</v>
+      </c>
+      <c r="F4" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,F$1)</f>
+        <v>50806730</v>
+      </c>
+      <c r="G4" s="7">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,G$1)</f>
+        <v>63246530</v>
+      </c>
+      <c r="H4" s="7">
+        <f>SUM(tabla_regiones[[#This Row],[Capioli]:[Zuloaga]])</f>
+        <v>576702901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,B$1)</f>
+        <v>135280108</v>
+      </c>
+      <c r="C5" s="7">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,C$1)</f>
+        <v>109144041</v>
+      </c>
+      <c r="D5" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,D$1)</f>
+        <v>94535993</v>
+      </c>
+      <c r="E5" s="7">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,E$1)</f>
+        <v>193222871</v>
+      </c>
+      <c r="F5" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,F$1)</f>
+        <v>48593995</v>
+      </c>
+      <c r="G5" s="7">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,G$1)</f>
+        <v>59797810</v>
+      </c>
+      <c r="H5" s="7">
+        <f>SUM(tabla_regiones[[#This Row],[Capioli]:[Zuloaga]])</f>
+        <v>640574818</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,B$1)</f>
+        <v>27153333</v>
+      </c>
+      <c r="C6" s="7">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,C$1)</f>
+        <v>232698504</v>
+      </c>
+      <c r="D6" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,D$1)</f>
+        <v>77744662</v>
+      </c>
+      <c r="E6" s="7">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,E$1)</f>
+        <v>131950052</v>
+      </c>
+      <c r="F6" s="3">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,F$1)</f>
+        <v>167729464</v>
+      </c>
+      <c r="G6" s="7">
+        <f>SUMIFS(ventas_precio,ventas_region,tabla_regiones[[#This Row],[Region]],ventas_vendedor,G$1)</f>
+        <v>40433106</v>
+      </c>
+      <c r="H6" s="7">
+        <f>SUM(tabla_regiones[[#This Row],[Capioli]:[Zuloaga]])</f>
+        <v>677709121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="7">
+        <f>SUBTOTAL(109,tabla_regiones[Capioli])</f>
+        <v>357852119</v>
+      </c>
+      <c r="C7" s="7">
+        <f>SUBTOTAL(109,tabla_regiones[Cardenas])</f>
+        <v>636402542</v>
+      </c>
+      <c r="D7" s="7">
+        <f>SUBTOTAL(109,tabla_regiones[Juarez])</f>
+        <v>712437428</v>
+      </c>
+      <c r="E7" s="7">
+        <f>SUBTOTAL(109,tabla_regiones[Lujan])</f>
+        <v>761464717</v>
+      </c>
+      <c r="F7" s="7">
+        <f>SUBTOTAL(109,tabla_regiones[Sanchez])</f>
+        <v>559356590</v>
+      </c>
+      <c r="G7" s="7">
+        <f>SUBTOTAL(109,tabla_regiones[Zuloaga])</f>
+        <v>226722785</v>
+      </c>
+      <c r="H7" s="7">
+        <f>SUBTOTAL(109,tabla_regiones[Total])</f>
+        <v>3254236181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -6694,12 +8165,25 @@
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181"/>
     </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:A6" xr:uid="{49FA5DA4-F2E8-4268-9AB4-039274B82003}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A6">
-      <sortCondition ref="A1:A6"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BE1901EA-C98C-4010-A4C4-32D65F8114C7}">
+          <x14:formula1>
+            <xm:f>vendedores!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:G1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>